<commit_message>
Error in Sheet Naming. Fixed
</commit_message>
<xml_diff>
--- a/data/Math_89_Ploomber.xlsx
+++ b/data/Math_89_Ploomber.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet r:id="rId1" sheetId="1" name="B1"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -135,7 +135,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,12 +153,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -216,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,7 +218,7 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -233,19 +227,16 @@
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -556,10 +547,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
@@ -656,7 +647,7 @@
       <c r="C7" s="4">
         <v>28</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="4">
         <f>ROUND(C7/35*100,2)</f>
       </c>
     </row>
@@ -810,7 +801,7 @@
       <c r="C18" s="4">
         <v>21</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="4">
         <f>ROUND(C18/35*100,2)</f>
       </c>
     </row>
@@ -950,7 +941,7 @@
       <c r="C28" s="4">
         <v>14</v>
       </c>
-      <c r="D28" s="7">
+      <c r="D28" s="4">
         <f>ROUND(C28/35*100,2)</f>
       </c>
     </row>
@@ -964,7 +955,7 @@
       <c r="C29" s="4">
         <v>14</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="4">
         <f>ROUND(C29/35*100,2)</f>
       </c>
     </row>

</xml_diff>